<commit_message>
Ajout des fichiers manquants et modifications nécessaires
</commit_message>
<xml_diff>
--- a/Tesst_But.xlsx
+++ b/Tesst_But.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr\Desktop\ligue1-visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275E6129-2B25-4936-B976-578AD76B5FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7F6B72-2F84-446E-8AAE-ACE9B3C3378C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{010B1BFA-5D63-4631-B649-FF082519AC4D}"/>
+    <workbookView xWindow="2138" yWindow="2213" windowWidth="16875" windowHeight="10522" xr2:uid="{010B1BFA-5D63-4631-B649-FF082519AC4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,6 @@
     <t>Joueur</t>
   </si>
   <si>
-    <t>Messi</t>
-  </si>
-  <si>
-    <t>Taha</t>
-  </si>
-  <si>
     <t>Anouar</t>
   </si>
   <si>
@@ -49,6 +43,12 @@
   </si>
   <si>
     <t>Karim</t>
+  </si>
+  <si>
+    <t>Montacer</t>
+  </si>
+  <si>
+    <t>Yassine</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -416,7 +416,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -435,7 +435,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -446,7 +446,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -479,7 +479,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -490,7 +490,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -501,7 +501,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -512,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -534,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -545,7 +545,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -556,7 +556,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -567,7 +567,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -578,7 +578,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -589,7 +589,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -600,7 +600,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>2</v>

</xml_diff>

<commit_message>
Ajout de la version avec filtres, résumé et annotations
</commit_message>
<xml_diff>
--- a/Tesst_But.xlsx
+++ b/Tesst_But.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr\Desktop\ligue1-visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7F6B72-2F84-446E-8AAE-ACE9B3C3378C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC467D-069D-4B1A-AF0C-BCB59E526DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2138" yWindow="2213" windowWidth="16875" windowHeight="10522" xr2:uid="{010B1BFA-5D63-4631-B649-FF082519AC4D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{010B1BFA-5D63-4631-B649-FF082519AC4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Match</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>Yassine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayoub </t>
+  </si>
+  <si>
+    <t>Amine</t>
+  </si>
+  <si>
+    <t>Yanis</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Salim</t>
+  </si>
+  <si>
+    <t>Rayane</t>
+  </si>
+  <si>
+    <t>Sebastien</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>Julien</t>
   </si>
 </sst>
 </file>
@@ -400,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4185C912-22A4-4500-800E-FDF7957E9C68}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -435,10 +462,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -457,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -482,7 +509,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -501,10 +528,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -515,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -537,7 +564,7 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -592,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -604,6 +631,127 @@
       </c>
       <c r="C18">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>